<commit_message>
re-ran analyses with slight plotting updates
</commit_message>
<xml_diff>
--- a/analyses/power analyses and meta analysis tables.xlsx
+++ b/analyses/power analyses and meta analysis tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/reanalysis-of-vahey-2015/manuscript/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian-Hussey/git/reanalysis-of-vahey-2015/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2989251-7C5D-0A4E-AA40-FF4A44B4C0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E33D65A-0823-D64A-81C8-145C455A48E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" activeTab="1" xr2:uid="{1835FDAE-4C49-9F48-9B57-DE64D2D554F2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Point estimate</t>
   </si>
@@ -131,9 +131,6 @@
     <t>Correction to set variance in population correlations to zero if it is negative, as in "h_s_ syntax.sps"</t>
   </si>
   <si>
-    <t>Correction to set variance in population correlations to zero if it is negative, as in "h_s_ syntax.sps", inapprorpriate Overton transformations removed</t>
-  </si>
-  <si>
     <t>Not calculated</t>
   </si>
   <si>
@@ -146,15 +143,6 @@
     <t>Verification attempt 2: Hunter &amp; Schmidt method (implementation 2)</t>
   </si>
   <si>
-    <t>Verification attempt 3: Hunter &amp; Schmidt method (implementation 2)</t>
-  </si>
-  <si>
-    <t>Verification attempt 4: Hunter &amp; Schmidt method (implementation 3)</t>
-  </si>
-  <si>
-    <t>Verification attempt 5: Mix of Hunter &amp; Schmidt and Hedges' methods</t>
-  </si>
-  <si>
     <t>Field &amp; Gillett's (2010) Basic meta-analysis</t>
   </si>
   <si>
@@ -168,6 +156,12 @@
   </si>
   <si>
     <t>Credibility intervals were implemented using Field &amp; Gillett's (2010) equations, Fisher's r-to-z transformations prior to analysis and z-to-r back transformations prior to reporting</t>
+  </si>
+  <si>
+    <t>Verification attempt 3: Hunter &amp; Schmidt method (implementation 3)</t>
+  </si>
+  <si>
+    <t>Verification attempt 4: Mix of Hunter &amp; Schmidt and Hedges' methods</t>
   </si>
 </sst>
 </file>
@@ -241,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -261,10 +255,8 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -295,9 +287,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -335,7 +327,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -441,7 +433,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -583,7 +575,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -594,7 +586,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,7 +647,7 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>0.45</v>
       </c>
       <c r="E3">
@@ -664,10 +656,10 @@
       <c r="F3">
         <v>29</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>0.18</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3">
         <v>189</v>
       </c>
     </row>
@@ -681,7 +673,7 @@
       <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>0.4</v>
       </c>
       <c r="E4">
@@ -690,10 +682,10 @@
       <c r="F4">
         <v>37</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>0.1</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4">
         <v>617</v>
       </c>
     </row>
@@ -707,7 +699,7 @@
       <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>0.45</v>
       </c>
       <c r="E5">
@@ -716,10 +708,10 @@
       <c r="F5">
         <v>36</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>0.18</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5">
         <v>240</v>
       </c>
     </row>
@@ -733,16 +725,16 @@
       <c r="C6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>0.4</v>
       </c>
       <c r="F6">
         <v>46</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>0.1</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6">
         <v>782</v>
       </c>
     </row>
@@ -756,7 +748,7 @@
       <c r="C7" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7">
         <v>1.01</v>
       </c>
       <c r="E7">
@@ -765,10 +757,10 @@
       <c r="F7">
         <v>26</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="8">
         <v>0.37</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7">
         <v>188</v>
       </c>
     </row>
@@ -782,19 +774,19 @@
       <c r="C8" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8">
         <v>0.87</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>36</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>34</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="8">
         <v>0.2</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8">
         <v>614</v>
       </c>
     </row>
@@ -808,7 +800,7 @@
       <c r="C9" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9">
         <v>1.01</v>
       </c>
       <c r="E9">
@@ -817,10 +809,10 @@
       <c r="F9">
         <v>8</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="8">
         <v>0.37</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9">
         <v>48</v>
       </c>
     </row>
@@ -834,7 +826,7 @@
       <c r="C10" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10">
         <v>0.87</v>
       </c>
       <c r="E10">
@@ -843,10 +835,10 @@
       <c r="F10">
         <v>10</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="8">
         <v>0.2</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10">
         <v>155</v>
       </c>
     </row>
@@ -865,10 +857,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4930379-F378-9D4C-A870-F0AD0F86B1AA}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -920,7 +912,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="4">
         <v>0.45</v>
@@ -939,11 +931,11 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>33</v>
+      <c r="A4" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -951,13 +943,13 @@
       <c r="D4" s="5">
         <v>0.47</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="9">
         <v>0.2</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <v>0.74</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="11">
         <v>0.47</v>
       </c>
       <c r="H4" s="5">
@@ -966,65 +958,65 @@
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="12">
         <v>0.46</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="14">
+      <c r="E5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="12">
         <v>0.46</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="12">
         <v>0.46</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.47</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.54</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0.47</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="14">
-        <v>0.47</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="14">
-        <v>0.47</v>
-      </c>
-      <c r="H6" s="14">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D7" s="5">
         <v>0.47</v>
@@ -1035,38 +1027,17 @@
       <c r="F7" s="6">
         <v>0.54</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="11">
         <v>0.47</v>
       </c>
       <c r="H7" s="5">
         <v>0.47</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.47</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="F8" s="6">
-        <v>0.54</v>
-      </c>
-      <c r="G8" s="13">
-        <v>0.47</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0.47</v>
-      </c>
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -1088,11 +1059,6 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>